<commit_message>
Made dropdown field by BEM using SVG file as an arrow. Need to make it in css!
</commit_message>
<xml_diff>
--- a/BEM.xlsx
+++ b/BEM.xlsx
@@ -71,6 +71,7 @@
   <si>
     <t xml:space="preserve">В фокусе:
 Рамка полупрозрачная,
+Убрать все стоковые обводки
 </t>
   </si>
 </sst>
@@ -88,12 +89,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,17 +115,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -148,8 +156,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>539927</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -451,7 +459,7 @@
   <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,13 +485,13 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
@@ -491,60 +499,60 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="2"/>
       <c r="E4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
+      <c r="B16" s="3"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
@@ -562,9 +570,10 @@
       <c r="B21" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B3:B11"/>
     <mergeCell ref="D3:D6"/>
+    <mergeCell ref="B13:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Remade dropdown field arrows. Made them in css
</commit_message>
<xml_diff>
--- a/BEM.xlsx
+++ b/BEM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>БЛОК</t>
   </si>
@@ -60,12 +60,6 @@
 Цвет текста почти темный</t>
   </si>
   <si>
-    <t>Правое поле:
-Абсол-е поз-е,
-Ширина 100% высоты блока,
-Позиционирование по центру</t>
-  </si>
-  <si>
     <t>Стрелка вправо градиентная</t>
   </si>
   <si>
@@ -73,6 +67,15 @@
 Рамка полупрозрачная,
 Убрать все стоковые обводки
 </t>
+  </si>
+  <si>
+    <t>Правое поле:
+Абсол-е поз-е,
+Ширина 100% высоты блока,
+flex</t>
+  </si>
+  <si>
+    <t>Стрелка вверх</t>
   </si>
 </sst>
 </file>
@@ -120,13 +123,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -459,7 +462,7 @@
   <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,11 +491,11 @@
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -500,27 +503,30 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="4"/>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="4"/>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
@@ -542,7 +548,7 @@
     </row>
     <row r="13" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UIkit blocks setup using BEM. United radio and checkboxes using mixins
</commit_message>
<xml_diff>
--- a/BEM.xlsx
+++ b/BEM.xlsx
@@ -462,7 +462,7 @@
   <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +497,7 @@
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -507,7 +507,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -517,7 +517,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>